<commit_message>
TS Kramam Tamil 5.1 and 5.2 22/12/2021
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Template Input Conf.xlsx
+++ b/TS Jatai Working/Raja Files/Template Input Conf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\texts\TS Jatai Working\Raja Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7EC822-76FB-4A8B-B0F3-C8ABA6B72672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D654F3B2-7A55-456C-BB0D-8F9B72EE8EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{570D827F-F0E0-4FE2-AA2E-C0DA2F43791E}"/>
   </bookViews>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7386C2B5-DBC7-42A8-B53B-6130EAEFF7CE}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>

</xml_diff>